<commit_message>
Polly error handling added
</commit_message>
<xml_diff>
--- a/PuppeteerApp/Data/DONE/Competitions_done_example.xlsx
+++ b/PuppeteerApp/Data/DONE/Competitions_done_example.xlsx
@@ -28,7 +28,7 @@
     <t>Premier League</t>
   </si>
   <si>
-    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\1_Premier League_2024-08-23-12-12-38.csv</t>
+    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\1_Premier League_2024-08-23-12-45-28.csv</t>
   </si>
   <si>
     <t>2.</t>
@@ -37,7 +37,7 @@
     <t>Division Profesional</t>
   </si>
   <si>
-    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\2_Division Profesional_2024-08-23-12-12-46.csv</t>
+    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\2_Division Profesional_2024-08-23-12-45-35.csv</t>
   </si>
   <si>
     <t>3.</t>
@@ -46,7 +46,7 @@
     <t>Ligue 1</t>
   </si>
   <si>
-    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\3_Ligue 1_2024-08-23-12-12-54.csv</t>
+    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\3_Ligue 1_2024-08-23-12-45-42.csv</t>
   </si>
   <si>
     <t>4.</t>
@@ -55,7 +55,7 @@
     <t>LaLiga</t>
   </si>
   <si>
-    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\4_LaLiga_2024-08-23-12-13-02.csv</t>
+    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\4_LaLiga_2024-08-23-12-45-49.csv</t>
   </si>
   <si>
     <t>5.</t>
@@ -64,7 +64,7 @@
     <t>Bundesliga</t>
   </si>
   <si>
-    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\5_Bundesliga_2024-08-23-12-13-10.csv</t>
+    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\5_Bundesliga_2024-08-23-12-45-57.csv</t>
   </si>
   <si>
     <t>6.</t>
@@ -73,26 +73,26 @@
     <t>Ekstraklasa</t>
   </si>
   <si>
-    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\6_Ekstraklasa_2024-08-23-12-13-17.csv</t>
+    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\6_Ekstraklasa_2024-08-23-12-46-14.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">Not enough values in row for team: AZS UŚ Katowice
-Not enough values in row for team: Rekord Bielsko-Biała
-Not enough values in row for team: Ruda Śląska
-Not enough values in row for team: FC Toruń
-Not enough values in row for team: Red Devils Chojnice
-Not enough values in row for team: Red Dragons Pniewy
-Not enough values in row for team: AZS Warszawa
-Not enough values in row for team: Piast Gliwice
-Not enough values in row for team: GI Malepszy Leszno
-Not enough values in row for team: Constract Lubawa
-Not enough values in row for team: Dreman Opole
-Not enough values in row for team: Widzew Łódź
-Not enough values in row for team: Legia Warszawa
-Not enough values in row for team: Bochnia
-Not enough values in row for team: Kamienica Krolewska
-Not enough values in row for team: Eurobus Przemysl
-No data found for competition: Ekstraklasa</t>
+    <t xml:space="preserve">Not enough values in row for team: AZS UŚ Katowice 
+Not enough values in row for team: Rekord Bielsko-Biała 
+Not enough values in row for team: Ruda Śląska 
+Not enough values in row for team: FC Toruń 
+Not enough values in row for team: Red Devils Chojnice 
+Not enough values in row for team: Red Dragons Pniewy 
+Not enough values in row for team: AZS Warszawa 
+Not enough values in row for team: Piast Gliwice 
+Not enough values in row for team: GI Malepszy Leszno 
+Not enough values in row for team: Constract Lubawa 
+Not enough values in row for team: Dreman Opole 
+Not enough values in row for team: Widzew Łódź 
+Not enough values in row for team: Legia Warszawa 
+Not enough values in row for team: Bochnia 
+Not enough values in row for team: Kamienica Krolewska 
+Not enough values in row for team: Eurobus Przemysl 
+No data found for competition: Ekstraklasa </t>
   </si>
   <si>
     <t>7.</t>
@@ -101,7 +101,7 @@
     <t>Serie A</t>
   </si>
   <si>
-    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\7_Serie A_2024-08-23-12-13-25.csv</t>
+    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\7_Serie A_2024-08-23-12-46-22.csv</t>
   </si>
   <si>
     <t>8.</t>
@@ -110,7 +110,7 @@
     <t>Betclic 1. Liga</t>
   </si>
   <si>
-    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\8_Betclic 1. Liga_2024-08-23-12-13-33.csv</t>
+    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\8_Betclic 1. Liga_2024-08-23-12-46-29.csv</t>
   </si>
   <si>
     <t>9.</t>
@@ -119,7 +119,7 @@
     <t>Wyszejszaja Liha</t>
   </si>
   <si>
-    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\9_Wyszejszaja Liha_2024-08-23-12-13-41.csv</t>
+    <t>C:\Users\Hubert\source\repos\PuppeteerApp\PuppeteerApp\Data/STANDINGS\9_Wyszejszaja Liha_2024-08-23-12-46-36.csv</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>